<commit_message>
add missing xslx changes
</commit_message>
<xml_diff>
--- a/data/shared_lost_genes.xlsx
+++ b/data/shared_lost_genes.xlsx
@@ -475,7 +475,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ventricular cardiac muscle cell action potential</t>
+          <t>positive regulation of potassium ion transmembrane transporter activity</t>
         </is>
       </c>
     </row>
@@ -485,7 +485,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>positive regulation of potassium ion transmembrane transporter activity</t>
+          <t>positive regulation of cation channel activity</t>
         </is>
       </c>
     </row>
@@ -495,7 +495,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>positive regulation of cation channel activity</t>
+          <t>ventricular cardiac muscle cell action potential</t>
         </is>
       </c>
     </row>
@@ -505,7 +505,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>regulation of atrial cardiac muscle cell action potential</t>
+          <t>membrane depolarization during SA node cell action potential</t>
         </is>
       </c>
     </row>
@@ -515,7 +515,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>membrane depolarization during SA node cell action potential</t>
+          <t>regulation of atrial cardiac muscle cell action potential</t>
         </is>
       </c>
     </row>
@@ -525,7 +525,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>regulation of SA node cell action potential</t>
+          <t>regulation of heart rate by cardiac conduction</t>
         </is>
       </c>
     </row>
@@ -535,7 +535,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>regulation of heart rate by cardiac conduction</t>
+          <t>regulation of SA node cell action potential</t>
         </is>
       </c>
     </row>
@@ -615,7 +615,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>negative regulation of vernalization response</t>
+          <t>regulation of membrane permeability</t>
         </is>
       </c>
     </row>
@@ -625,7 +625,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>response to herbivore</t>
+          <t>negative regulation of vernalization response</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>response to molecule of fungal origin</t>
+          <t>response to herbivore</t>
         </is>
       </c>
     </row>
@@ -645,7 +645,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>protein localization to cell surface</t>
+          <t>response to molecule of fungal origin</t>
         </is>
       </c>
     </row>
@@ -655,7 +655,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>regulation of membrane permeability</t>
+          <t>protein localization to cell surface</t>
         </is>
       </c>
     </row>
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>photoreceptor cell outer segment organization</t>
+          <t>retinal rod cell development</t>
         </is>
       </c>
     </row>
@@ -1175,7 +1175,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>retinal rod cell development</t>
+          <t>photoreceptor cell outer segment organization</t>
         </is>
       </c>
     </row>

</xml_diff>